<commit_message>
update UI of chatbot
</commit_message>
<xml_diff>
--- a/source/infrastructure/lib/api/asset/intention_corpus.xlsx
+++ b/source/infrastructure/lib/api/asset/intention_corpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuihubin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCE6895-E699-5248-835E-B80A5E8FB3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B558B0F-CEB2-3545-951A-1E92977EFCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{469B79FB-39B9-9946-996E-61F15C850FAB}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <author>Cui, Hubin</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A6EA9CB1-5D1E-FB40-8DE4-4B8049EC6F86}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{4C306300-7FAC-7640-AF12-F4F6E2F8BFA5}">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Cui, Hubin:</t>
+          <t>aics:</t>
         </r>
         <r>
           <rPr>
@@ -64,49 +64,45 @@
         </r>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>eg</t>
+          <t xml:space="preserve">eg: </t>
         </r>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-          </rPr>
-          <t>:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t>a=1,b=2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -115,19 +111,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>question</t>
   </si>
   <si>
     <t>intention</t>
   </si>
+  <si>
+    <t>kwargs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +152,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -521,83 +527,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6966AB3-4EDE-2747-88FD-B9A9AF53C030}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="81.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>